<commit_message>
Untar image bundle images
I left the original formatted.tar.gz in place.
I added the files to the spreadsheet assay and files tabs, but I did not complete all the assay info.  I'm not sure what to put there.
</commit_message>
<xml_diff>
--- a/2017-10/image/Q3Demo_Imaging.xlsx
+++ b/2017-10/image/Q3Demo_Imaging.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupp/dev/hca/demo-data/2017-10/imaging/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sampierson/Development/HCA/demo-data/2017-10/image/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="3840" windowWidth="27460" windowHeight="17460" activeTab="6"/>
+    <workbookView xWindow="5860" yWindow="3840" windowWidth="27460" windowHeight="17460" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>title</t>
   </si>
@@ -206,6 +206,69 @@
   </si>
   <si>
     <t>"formatted.tar.gz"</t>
+  </si>
+  <si>
+    <t>fov_0_H_0_C_0.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_0_C_1.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_0_C_2.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_0_C_3.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_1_C_0.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_1_C_1.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_1_C_2.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_1_C_3.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_2_C_0.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_2_C_1.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_2_C_2.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_2_C_3.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_3_C_0.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_3_C_1.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_3_C_2.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_H_3_C_3.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_dapi.tiff</t>
+  </si>
+  <si>
+    <t>fov_0_dots.tiff</t>
+  </si>
+  <si>
+    <t>.tiff</t>
+  </si>
+  <si>
+    <t>org.json</t>
+  </si>
+  <si>
+    <t>.json</t>
   </si>
 </sst>
 </file>
@@ -871,10 +934,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="G1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -959,6 +1022,101 @@
       </c>
       <c r="J2" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -987,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1014,6 +1172,158 @@
         <v>35</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updated assay metadata for imaging files
</commit_message>
<xml_diff>
--- a/2017-10/image/Q3Demo_Imaging.xlsx
+++ b/2017-10/image/Q3Demo_Imaging.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sampierson/Development/HCA/demo-data/2017-10/image/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupp/dev/hca/demo-data/2017-10/image/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="3840" windowWidth="27460" windowHeight="17460" activeTab="8"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="27460" windowHeight="17460" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>title</t>
   </si>
@@ -205,9 +205,6 @@
     <t>files</t>
   </si>
   <si>
-    <t>"formatted.tar.gz"</t>
-  </si>
-  <si>
     <t>fov_0_H_0_C_0.tiff</t>
   </si>
   <si>
@@ -269,6 +266,9 @@
   </si>
   <si>
     <t>.json</t>
+  </si>
+  <si>
+    <t>fov_0_H_0_C_0.tiff || fov_0_H_0_C_1.tiff || fov_0_H_0_C_2.tiff || fov_0_H_0_C_3.tiff || fov_0_H_1_C_0.tiff || fov_0_H_1_C_1.tiff || fov_0_H_1_C_2.tiff || fov_0_H_1_C_3.tiff || fov_0_H_2_C_0.tiff || fov_0_H_2_C_1.tiff || fov_0_H_2_C_2.tiff || fov_0_H_2_C_3.tiff || fov_0_H_3_C_0.tiff || fov_0_H_3_C_1.tiff || fov_0_H_3_C_2.tiff || fov_0_H_3_C_3.tiff || fov_0_dapi.tiff || fov_0_dots.tiff || org.json</t>
   </si>
 </sst>
 </file>
@@ -934,10 +934,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1021,102 +1021,7 @@
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1147,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -1174,154 +1079,154 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
         <v>76</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>